<commit_message>
Baseline Wandering Cleared outputs
</commit_message>
<xml_diff>
--- a/outputs/tables/confusion matrices.xlsx
+++ b/outputs/tables/confusion matrices.xlsx
@@ -577,10 +577,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>797</v>
@@ -609,10 +609,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E5" t="n">
         <v>9</v>
@@ -645,10 +645,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
         <v>788</v>
@@ -745,10 +745,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" t="n">
         <v>3</v>
@@ -781,10 +781,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
         <v>808</v>
@@ -813,10 +813,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -881,10 +881,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E13" t="n">
         <v>3</v>
@@ -917,10 +917,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>789</v>
@@ -949,10 +949,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E15" t="n">
         <v>7</v>

</xml_diff>